<commit_message>
Generación de archivo final de asistentes
</commit_message>
<xml_diff>
--- a/Archivo de prueba Google forms.xlsx
+++ b/Archivo de prueba Google forms.xlsx
@@ -24,15 +24,9 @@
     <t>Marca temporal</t>
   </si>
   <si>
-    <t>Dirección de correo electrónico</t>
-  </si>
-  <si>
     <t>Nombre Completo</t>
   </si>
   <si>
-    <t>Tipo de identificación</t>
-  </si>
-  <si>
     <t>Empresa y/o profesión y/o actividad</t>
   </si>
   <si>
@@ -412,6 +406,12 @@
   </si>
   <si>
     <t>Numero de identificacion</t>
+  </si>
+  <si>
+    <t>Tipo de identificacion</t>
+  </si>
+  <si>
+    <t>Direccion de correo electronico</t>
   </si>
 </sst>
 </file>
@@ -753,7 +753,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -773,1537 +773,1537 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <f ca="1">TODAY()</f>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <f ca="1">INT(RAND()*10^10)</f>
-        <v>32852952</v>
+        <v>97809442</v>
       </c>
       <c r="F2" t="str">
         <f ca="1">CONCATENATE("3",INT(RAND()*10^9))</f>
-        <v>3460033270</v>
+        <v>3522272752</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <f t="shared" ref="A3:A60" ca="1" si="0">TODAY()</f>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E60" ca="1" si="1">INT(RAND()*10^10)</f>
-        <v>2781117491</v>
+        <v>4296043792</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F60" ca="1" si="2">CONCATENATE("3",INT(RAND()*10^9))</f>
-        <v>3323262478</v>
+        <v>3477962835</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>4434560597</v>
+        <v>9081966526</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3769575617</v>
+        <v>3356395359</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>4901797033</v>
+        <v>8124938316</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3443209650</v>
+        <v>3598186428</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>6091347282</v>
+        <v>5163725943</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3415165944</v>
+        <v>3993026342</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>3912289812</v>
+        <v>1009847997</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3190426757</v>
+        <v>3925176339</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="1"/>
+        <v>1050956926</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>3124283150</v>
+      </c>
+      <c r="G8" t="s">
         <v>5</v>
-      </c>
-      <c r="E8">
-        <f t="shared" ca="1" si="1"/>
-        <v>2902730134</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3442623676</v>
-      </c>
-      <c r="G8" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>2446096286</v>
+        <v>1435590564</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3773521538</v>
+        <v>3763350664</v>
       </c>
       <c r="G9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>7350862285</v>
+        <v>3309749681</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3454964570</v>
+        <v>3621995571</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>4868965576</v>
+        <v>2875948781</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3697109835</v>
+        <v>3802057992</v>
       </c>
       <c r="G11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="1"/>
-        <v>4389839237</v>
+        <v>2088504113</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3901748919</v>
+        <v>3733846325</v>
       </c>
       <c r="G12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="1"/>
-        <v>9179546566</v>
+        <v>5211507119</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3998656035</v>
+        <v>3961481703</v>
       </c>
       <c r="G13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ca="1" si="1"/>
+        <v>306099357</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>3818873221</v>
+      </c>
+      <c r="G14" t="s">
         <v>5</v>
-      </c>
-      <c r="E14">
-        <f t="shared" ca="1" si="1"/>
-        <v>525568533</v>
-      </c>
-      <c r="F14" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3659187166</v>
-      </c>
-      <c r="G14" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="1"/>
-        <v>2317038901</v>
+        <v>2351065360</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3424635667</v>
+        <v>3917215280</v>
       </c>
       <c r="G15" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ca="1" si="1"/>
+        <v>841820231</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>3879274286</v>
+      </c>
+      <c r="G16" t="s">
         <v>38</v>
-      </c>
-      <c r="D16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16">
-        <f t="shared" ca="1" si="1"/>
-        <v>9904831252</v>
-      </c>
-      <c r="F16" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3722802826</v>
-      </c>
-      <c r="G16" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>8332608647</v>
+        <v>1045860950</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3144377642</v>
+        <v>3673668097</v>
       </c>
       <c r="G17" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>9947920974</v>
+        <v>5779330048</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3221679966</v>
+        <v>3137857888</v>
       </c>
       <c r="G18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D19" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>9662962700</v>
+        <v>8964761110</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3917382499</v>
+        <v>3908113562</v>
       </c>
       <c r="G19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>5155861065</v>
+        <v>8394803070</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3672970993</v>
+        <v>3315388829</v>
       </c>
       <c r="G20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>5727078700</v>
+        <v>2915624850</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3963304933</v>
+        <v>3205419789</v>
       </c>
       <c r="G21" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ca="1" si="1"/>
+        <v>9700500596</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>317127368</v>
+      </c>
+      <c r="G22" t="s">
         <v>5</v>
-      </c>
-      <c r="E22">
-        <f t="shared" ca="1" si="1"/>
-        <v>5260883229</v>
-      </c>
-      <c r="F22" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>374075106</v>
-      </c>
-      <c r="G22" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D23" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>3652095305</v>
+        <v>2805764622</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3356326778</v>
+        <v>3188221344</v>
       </c>
       <c r="G23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D24" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>1776179505</v>
+        <v>7769248117</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3241729493</v>
+        <v>3483228283</v>
       </c>
       <c r="G24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>6113402034</v>
+        <v>8071029267</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>348450495</v>
+        <v>3934954877</v>
       </c>
       <c r="G25" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="1"/>
-        <v>5879100383</v>
+        <v>9401182304</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3266501648</v>
+        <v>3862241303</v>
       </c>
       <c r="G26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D27" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="1"/>
-        <v>2864459169</v>
+        <v>1419968243</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>355733325</v>
+        <v>3883359534</v>
       </c>
       <c r="G27" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D28" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="1"/>
-        <v>1813508319</v>
+        <v>5928326156</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3310584897</v>
+        <v>3463225246</v>
       </c>
       <c r="G28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="1"/>
-        <v>5859508187</v>
+        <v>2889860421</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3734041254</v>
+        <v>3640178220</v>
       </c>
       <c r="G29" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <f t="shared" ca="1" si="1"/>
+        <v>8155591887</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>3802100158</v>
+      </c>
+      <c r="G30" t="s">
         <v>5</v>
-      </c>
-      <c r="E30">
-        <f t="shared" ca="1" si="1"/>
-        <v>1118105739</v>
-      </c>
-      <c r="F30" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3341622409</v>
-      </c>
-      <c r="G30" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D31" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="1"/>
-        <v>7012089831</v>
+        <v>5742722230</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3938777248</v>
+        <v>3957150709</v>
       </c>
       <c r="G31" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D32" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="1"/>
-        <v>2240874652</v>
+        <v>2667232291</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3440313451</v>
+        <v>3563035012</v>
       </c>
       <c r="G32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D33" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="1"/>
-        <v>5142511945</v>
+        <v>7667388476</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3253487097</v>
+        <v>3660932592</v>
       </c>
       <c r="G33" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="1"/>
-        <v>7829113587</v>
+        <v>3163090632</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>356470375</v>
+        <v>3164283105</v>
       </c>
       <c r="G34" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D35" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="1"/>
-        <v>6662195212</v>
+        <v>5263730742</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3508116728</v>
+        <v>3388238880</v>
       </c>
       <c r="G35" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D36" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="1"/>
-        <v>7451319163</v>
+        <v>8360020056</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3428360587</v>
+        <v>3967055929</v>
       </c>
       <c r="G36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D37" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="1"/>
-        <v>6183028168</v>
+        <v>262338008</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>378200452</v>
+        <v>310741827</v>
       </c>
       <c r="G37" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B38" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38">
+        <f t="shared" ca="1" si="1"/>
+        <v>5827784171</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>397386755</v>
+      </c>
+      <c r="G38" t="s">
         <v>5</v>
-      </c>
-      <c r="E38">
-        <f t="shared" ca="1" si="1"/>
-        <v>3592128973</v>
-      </c>
-      <c r="F38" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>321955917</v>
-      </c>
-      <c r="G38" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D39" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E39">
         <f t="shared" ca="1" si="1"/>
-        <v>8535815651</v>
+        <v>1025851220</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3561445594</v>
+        <v>3493781406</v>
       </c>
       <c r="G39" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B40" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D40" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E40">
         <f t="shared" ca="1" si="1"/>
-        <v>4090128403</v>
+        <v>3528439780</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3736250482</v>
+        <v>3290347053</v>
       </c>
       <c r="G40" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:7" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C41" s="6"/>
     </row>
     <row r="42" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B42" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D42" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E42">
         <f t="shared" ca="1" si="1"/>
-        <v>3288938651</v>
+        <v>6376928469</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3375697304</v>
+        <v>3252295088</v>
       </c>
       <c r="G42" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B43" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D43" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E43">
         <f t="shared" ca="1" si="1"/>
-        <v>6220940339</v>
+        <v>5763593401</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>358235452</v>
+        <v>3852436766</v>
       </c>
       <c r="G43" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B44" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D44" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E44">
         <f t="shared" ca="1" si="1"/>
-        <v>3759911103</v>
+        <v>8812131200</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3179554625</v>
+        <v>3354562978</v>
       </c>
       <c r="G44" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B45" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D45" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E45">
         <f t="shared" ca="1" si="1"/>
-        <v>2464960870</v>
+        <v>2681130857</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3839519798</v>
+        <v>3926495203</v>
       </c>
       <c r="G45" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B46" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D46" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E46">
         <f t="shared" ca="1" si="1"/>
-        <v>4066250642</v>
+        <v>653180009</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3738464441</v>
+        <v>3390067327</v>
       </c>
       <c r="G46" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B47" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47">
+        <f t="shared" ca="1" si="1"/>
+        <v>6173337666</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>338233932</v>
+      </c>
+      <c r="G47" t="s">
         <v>5</v>
-      </c>
-      <c r="E47">
-        <f t="shared" ca="1" si="1"/>
-        <v>3478026424</v>
-      </c>
-      <c r="F47" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3687271892</v>
-      </c>
-      <c r="G47" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B48" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D48" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E48">
         <f t="shared" ca="1" si="1"/>
-        <v>5161731233</v>
+        <v>4379586803</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3846453831</v>
+        <v>314161341</v>
       </c>
       <c r="G48" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D49" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E49">
         <f t="shared" ca="1" si="1"/>
-        <v>4337799732</v>
+        <v>2085484989</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>371308400</v>
+        <v>3475292451</v>
       </c>
       <c r="G49" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B50" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D50" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E50">
         <f t="shared" ca="1" si="1"/>
-        <v>2898832048</v>
+        <v>8469382353</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3475091896</v>
+        <v>3834187320</v>
       </c>
       <c r="G50" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B51" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D51" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E51">
         <f t="shared" ca="1" si="1"/>
-        <v>9299618555</v>
+        <v>7145068514</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3445776301</v>
+        <v>3543787436</v>
       </c>
       <c r="G51" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D52" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E52">
         <f t="shared" ca="1" si="1"/>
-        <v>107054671</v>
+        <v>4947404582</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3415675926</v>
+        <v>3958262719</v>
       </c>
       <c r="G52" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B53" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D53" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E53">
         <f t="shared" ca="1" si="1"/>
-        <v>5742426451</v>
+        <v>2152264420</v>
       </c>
       <c r="F53" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3536639158</v>
+        <v>3857167077</v>
       </c>
       <c r="G53" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B54" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D54" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E54">
         <f t="shared" ca="1" si="1"/>
-        <v>3585903492</v>
+        <v>7276312916</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3896469460</v>
+        <v>3704849098</v>
       </c>
       <c r="G54" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B55" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D55" t="s">
+        <v>3</v>
+      </c>
+      <c r="E55">
+        <f t="shared" ca="1" si="1"/>
+        <v>7551894404</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>3202634534</v>
+      </c>
+      <c r="G55" t="s">
         <v>5</v>
-      </c>
-      <c r="E55">
-        <f t="shared" ca="1" si="1"/>
-        <v>6212728001</v>
-      </c>
-      <c r="F55" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>32289358</v>
-      </c>
-      <c r="G55" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D56" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E56">
         <f t="shared" ca="1" si="1"/>
-        <v>5002906512</v>
+        <v>1091702375</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3321842203</v>
+        <v>3360985502</v>
       </c>
       <c r="G56" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B57" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D57" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E57">
         <f t="shared" ca="1" si="1"/>
-        <v>3006198687</v>
+        <v>6260514936</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3594328751</v>
+        <v>3995407587</v>
       </c>
       <c r="G57" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B58" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D58" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E58">
         <f t="shared" ca="1" si="1"/>
-        <v>7242897303</v>
+        <v>948374570</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3531649018</v>
+        <v>3208685623</v>
       </c>
       <c r="G58" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D59" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E59">
         <f t="shared" ca="1" si="1"/>
-        <v>2555652676</v>
+        <v>5482407084</v>
       </c>
       <c r="F59" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3151048520</v>
+        <v>3553428714</v>
       </c>
       <c r="G59" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43940</v>
+        <v>43941</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D60" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E60">
         <f t="shared" ca="1" si="1"/>
-        <v>2264902460</v>
+        <v>7017477318</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>3216409505</v>
+        <v>3382046479</v>
       </c>
       <c r="G60" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Comparacion de archivos y generacion de dataframe resultante
</commit_message>
<xml_diff>
--- a/Archivo de prueba Google forms.xlsx
+++ b/Archivo de prueba Google forms.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Pybaq\SAR\sar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pandrearro\Documents\Python\sar\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -418,13 +418,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -457,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -466,6 +473,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -752,8 +760,8 @@
   <dimension ref="A1:G483"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -793,8 +801,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <f ca="1">TODAY()</f>
-        <v>43941</v>
+        <v>43900</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -807,11 +814,11 @@
       </c>
       <c r="E2">
         <f ca="1">INT(RAND()*10^10)</f>
-        <v>97809442</v>
+        <v>1660500432</v>
       </c>
       <c r="F2" t="str">
         <f ca="1">CONCATENATE("3",INT(RAND()*10^9))</f>
-        <v>3522272752</v>
+        <v>3827801515</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
@@ -819,8 +826,7 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <f t="shared" ref="A3:A60" ca="1" si="0">TODAY()</f>
-        <v>43941</v>
+        <v>43901</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -832,12 +838,12 @@
         <v>3</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E60" ca="1" si="1">INT(RAND()*10^10)</f>
-        <v>4296043792</v>
+        <f t="shared" ref="E3:E60" ca="1" si="0">INT(RAND()*10^10)</f>
+        <v>586519008</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F60" ca="1" si="2">CONCATENATE("3",INT(RAND()*10^9))</f>
-        <v>3477962835</v>
+        <f t="shared" ref="F3:F60" ca="1" si="1">CONCATENATE("3",INT(RAND()*10^9))</f>
+        <v>3233800728</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -845,8 +851,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43902</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -858,12 +863,12 @@
         <v>3</v>
       </c>
       <c r="E4">
-        <f t="shared" ca="1" si="1"/>
-        <v>9081966526</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2180241337</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3356395359</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3904423220</v>
       </c>
       <c r="G4" t="s">
         <v>38</v>
@@ -871,8 +876,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43903</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
@@ -884,12 +888,12 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <f t="shared" ca="1" si="1"/>
-        <v>8124938316</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1986524254</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3598186428</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>367809184</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
@@ -897,8 +901,7 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43904</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
@@ -910,12 +913,12 @@
         <v>3</v>
       </c>
       <c r="E6">
-        <f t="shared" ca="1" si="1"/>
-        <v>5163725943</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6527368838</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3993026342</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3430086797</v>
       </c>
       <c r="G6" t="s">
         <v>39</v>
@@ -923,8 +926,7 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43905</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -936,12 +938,12 @@
         <v>3</v>
       </c>
       <c r="E7">
-        <f t="shared" ca="1" si="1"/>
-        <v>1009847997</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3632313044</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3925176339</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3679649570</v>
       </c>
       <c r="G7" t="s">
         <v>7</v>
@@ -949,8 +951,7 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43906</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
@@ -962,12 +963,12 @@
         <v>3</v>
       </c>
       <c r="E8">
-        <f t="shared" ca="1" si="1"/>
-        <v>1050956926</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9632525407</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3124283150</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3606108895</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
@@ -975,8 +976,7 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43907</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
@@ -988,12 +988,12 @@
         <v>3</v>
       </c>
       <c r="E9">
-        <f t="shared" ca="1" si="1"/>
-        <v>1435590564</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7882395799</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3763350664</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3252152628</v>
       </c>
       <c r="G9" t="s">
         <v>4</v>
@@ -1001,8 +1001,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43908</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
@@ -1014,12 +1013,12 @@
         <v>3</v>
       </c>
       <c r="E10">
-        <f t="shared" ca="1" si="1"/>
-        <v>3309749681</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2883747785</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3621995571</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3478209133</v>
       </c>
       <c r="G10" t="s">
         <v>38</v>
@@ -1027,8 +1026,7 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43909</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
@@ -1040,12 +1038,12 @@
         <v>3</v>
       </c>
       <c r="E11">
-        <f t="shared" ca="1" si="1"/>
-        <v>2875948781</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7762150326</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3802057992</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3958937410</v>
       </c>
       <c r="G11" t="s">
         <v>6</v>
@@ -1053,8 +1051,7 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43910</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
@@ -1066,12 +1063,12 @@
         <v>3</v>
       </c>
       <c r="E12">
-        <f t="shared" ca="1" si="1"/>
-        <v>2088504113</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4914737174</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3733846325</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3290150402</v>
       </c>
       <c r="G12" t="s">
         <v>39</v>
@@ -1079,8 +1076,7 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43911</v>
       </c>
       <c r="B13" t="s">
         <v>31</v>
@@ -1092,12 +1088,12 @@
         <v>3</v>
       </c>
       <c r="E13">
-        <f t="shared" ca="1" si="1"/>
-        <v>5211507119</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2024994163</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3961481703</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3804174572</v>
       </c>
       <c r="G13" t="s">
         <v>7</v>
@@ -1105,8 +1101,7 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43912</v>
       </c>
       <c r="B14" t="s">
         <v>33</v>
@@ -1118,12 +1113,12 @@
         <v>3</v>
       </c>
       <c r="E14">
-        <f t="shared" ca="1" si="1"/>
-        <v>306099357</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>168531206</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3818873221</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3701003885</v>
       </c>
       <c r="G14" t="s">
         <v>5</v>
@@ -1131,8 +1126,7 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43913</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
@@ -1144,12 +1138,12 @@
         <v>3</v>
       </c>
       <c r="E15">
-        <f t="shared" ca="1" si="1"/>
-        <v>2351065360</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5413324726</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3917215280</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>36881275</v>
       </c>
       <c r="G15" t="s">
         <v>4</v>
@@ -1157,8 +1151,7 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43914</v>
       </c>
       <c r="B16" t="s">
         <v>37</v>
@@ -1170,12 +1163,12 @@
         <v>3</v>
       </c>
       <c r="E16">
-        <f t="shared" ca="1" si="1"/>
-        <v>841820231</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>8893579456</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3879274286</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3487800354</v>
       </c>
       <c r="G16" t="s">
         <v>38</v>
@@ -1183,8 +1176,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43915</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>49</v>
@@ -1196,12 +1188,12 @@
         <v>3</v>
       </c>
       <c r="E17">
-        <f t="shared" ca="1" si="1"/>
-        <v>1045860950</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3352413859</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3673668097</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3589971452</v>
       </c>
       <c r="G17" t="s">
         <v>4</v>
@@ -1209,8 +1201,7 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43916</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>50</v>
@@ -1222,12 +1213,12 @@
         <v>3</v>
       </c>
       <c r="E18">
-        <f t="shared" ca="1" si="1"/>
-        <v>5779330048</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>8045748035</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3137857888</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3716452674</v>
       </c>
       <c r="G18" t="s">
         <v>38</v>
@@ -1235,8 +1226,7 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43917</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>51</v>
@@ -1248,12 +1238,12 @@
         <v>3</v>
       </c>
       <c r="E19">
-        <f t="shared" ca="1" si="1"/>
-        <v>8964761110</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9523354889</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3908113562</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3899832444</v>
       </c>
       <c r="G19" t="s">
         <v>6</v>
@@ -1261,8 +1251,7 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43918</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>52</v>
@@ -1274,12 +1263,12 @@
         <v>3</v>
       </c>
       <c r="E20">
-        <f t="shared" ca="1" si="1"/>
-        <v>8394803070</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3066600459</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3315388829</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3853467958</v>
       </c>
       <c r="G20" t="s">
         <v>39</v>
@@ -1287,8 +1276,7 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43919</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>53</v>
@@ -1300,12 +1288,12 @@
         <v>3</v>
       </c>
       <c r="E21">
-        <f t="shared" ca="1" si="1"/>
-        <v>2915624850</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7858263366</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3205419789</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3524756580</v>
       </c>
       <c r="G21" t="s">
         <v>7</v>
@@ -1313,8 +1301,7 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43920</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>85</v>
@@ -1326,12 +1313,12 @@
         <v>3</v>
       </c>
       <c r="E22">
-        <f t="shared" ca="1" si="1"/>
-        <v>9700500596</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>95300476</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>317127368</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3917382698</v>
       </c>
       <c r="G22" t="s">
         <v>5</v>
@@ -1339,8 +1326,7 @@
     </row>
     <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43921</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>86</v>
@@ -1352,12 +1338,12 @@
         <v>3</v>
       </c>
       <c r="E23">
-        <f t="shared" ca="1" si="1"/>
-        <v>2805764622</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7786225422</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3188221344</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3753689238</v>
       </c>
       <c r="G23" t="s">
         <v>4</v>
@@ -1365,8 +1351,7 @@
     </row>
     <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43891</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>54</v>
@@ -1378,12 +1363,12 @@
         <v>3</v>
       </c>
       <c r="E24">
-        <f t="shared" ca="1" si="1"/>
-        <v>7769248117</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7577342224</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3483228283</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3761653352</v>
       </c>
       <c r="G24" t="s">
         <v>38</v>
@@ -1391,8 +1376,7 @@
     </row>
     <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43892</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>87</v>
@@ -1404,12 +1388,12 @@
         <v>3</v>
       </c>
       <c r="E25">
-        <f t="shared" ca="1" si="1"/>
-        <v>8071029267</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6369233294</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3934954877</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3358430469</v>
       </c>
       <c r="G25" t="s">
         <v>4</v>
@@ -1417,8 +1401,7 @@
     </row>
     <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43893</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>55</v>
@@ -1430,12 +1413,12 @@
         <v>3</v>
       </c>
       <c r="E26">
-        <f t="shared" ca="1" si="1"/>
-        <v>9401182304</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9464153315</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3862241303</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3832155610</v>
       </c>
       <c r="G26" t="s">
         <v>38</v>
@@ -1443,8 +1426,7 @@
     </row>
     <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43894</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>56</v>
@@ -1456,12 +1438,12 @@
         <v>3</v>
       </c>
       <c r="E27">
-        <f t="shared" ca="1" si="1"/>
-        <v>1419968243</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4223998962</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3883359534</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3483425130</v>
       </c>
       <c r="G27" t="s">
         <v>6</v>
@@ -1469,8 +1451,7 @@
     </row>
     <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43895</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>88</v>
@@ -1482,12 +1463,12 @@
         <v>3</v>
       </c>
       <c r="E28">
-        <f t="shared" ca="1" si="1"/>
-        <v>5928326156</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6574724409</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3463225246</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3768103502</v>
       </c>
       <c r="G28" t="s">
         <v>39</v>
@@ -1495,8 +1476,7 @@
     </row>
     <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43896</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>89</v>
@@ -1508,12 +1488,12 @@
         <v>3</v>
       </c>
       <c r="E29">
-        <f t="shared" ca="1" si="1"/>
-        <v>2889860421</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6438959073</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3640178220</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>380338296</v>
       </c>
       <c r="G29" t="s">
         <v>7</v>
@@ -1521,8 +1501,7 @@
     </row>
     <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43897</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>90</v>
@@ -1534,12 +1513,12 @@
         <v>3</v>
       </c>
       <c r="E30">
-        <f t="shared" ca="1" si="1"/>
-        <v>8155591887</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7053111061</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3802100158</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3549473059</v>
       </c>
       <c r="G30" t="s">
         <v>5</v>
@@ -1547,8 +1526,7 @@
     </row>
     <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43898</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>91</v>
@@ -1560,12 +1538,12 @@
         <v>3</v>
       </c>
       <c r="E31">
-        <f t="shared" ca="1" si="1"/>
-        <v>5742722230</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3927292903</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3957150709</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3883904288</v>
       </c>
       <c r="G31" t="s">
         <v>4</v>
@@ -1573,8 +1551,7 @@
     </row>
     <row r="32" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43899</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>92</v>
@@ -1586,12 +1563,12 @@
         <v>3</v>
       </c>
       <c r="E32">
-        <f t="shared" ca="1" si="1"/>
-        <v>2667232291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7436438745</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3563035012</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>355264349</v>
       </c>
       <c r="G32" t="s">
         <v>38</v>
@@ -1599,8 +1576,7 @@
     </row>
     <row r="33" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43900</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>93</v>
@@ -1612,12 +1588,12 @@
         <v>3</v>
       </c>
       <c r="E33">
-        <f t="shared" ca="1" si="1"/>
-        <v>7667388476</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>8974633151</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3660932592</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3864163663</v>
       </c>
       <c r="G33" t="s">
         <v>4</v>
@@ -1625,8 +1601,7 @@
     </row>
     <row r="34" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43901</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>94</v>
@@ -1638,12 +1613,12 @@
         <v>3</v>
       </c>
       <c r="E34">
-        <f t="shared" ca="1" si="1"/>
-        <v>3163090632</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5461921631</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3164283105</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3668729882</v>
       </c>
       <c r="G34" t="s">
         <v>38</v>
@@ -1651,8 +1626,7 @@
     </row>
     <row r="35" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43902</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>95</v>
@@ -1664,12 +1638,12 @@
         <v>3</v>
       </c>
       <c r="E35">
-        <f t="shared" ca="1" si="1"/>
-        <v>5263730742</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9617140973</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3388238880</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3443169525</v>
       </c>
       <c r="G35" t="s">
         <v>6</v>
@@ -1677,8 +1651,7 @@
     </row>
     <row r="36" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43903</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>96</v>
@@ -1690,12 +1663,12 @@
         <v>3</v>
       </c>
       <c r="E36">
-        <f t="shared" ca="1" si="1"/>
-        <v>8360020056</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4816803916</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3967055929</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3284733345</v>
       </c>
       <c r="G36" t="s">
         <v>39</v>
@@ -1703,8 +1676,7 @@
     </row>
     <row r="37" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43904</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>97</v>
@@ -1716,12 +1688,12 @@
         <v>3</v>
       </c>
       <c r="E37">
-        <f t="shared" ca="1" si="1"/>
-        <v>262338008</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>530963254</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>310741827</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3219973360</v>
       </c>
       <c r="G37" t="s">
         <v>7</v>
@@ -1729,8 +1701,7 @@
     </row>
     <row r="38" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43905</v>
       </c>
       <c r="B38" t="s">
         <v>98</v>
@@ -1742,12 +1713,12 @@
         <v>3</v>
       </c>
       <c r="E38">
-        <f t="shared" ca="1" si="1"/>
-        <v>5827784171</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1490896138</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>397386755</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3454663952</v>
       </c>
       <c r="G38" t="s">
         <v>5</v>
@@ -1755,8 +1726,7 @@
     </row>
     <row r="39" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43906</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>70</v>
@@ -1768,12 +1738,12 @@
         <v>3</v>
       </c>
       <c r="E39">
-        <f t="shared" ca="1" si="1"/>
-        <v>1025851220</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>8023682847</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3493781406</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3355260176</v>
       </c>
       <c r="G39" t="s">
         <v>4</v>
@@ -1781,8 +1751,7 @@
     </row>
     <row r="40" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43907</v>
       </c>
       <c r="B40" t="s">
         <v>99</v>
@@ -1794,12 +1763,12 @@
         <v>3</v>
       </c>
       <c r="E40">
-        <f t="shared" ca="1" si="1"/>
-        <v>3528439780</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>8337895046</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3290347053</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>337929756</v>
       </c>
       <c r="G40" t="s">
         <v>38</v>
@@ -1814,8 +1783,7 @@
     </row>
     <row r="42" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43923</v>
       </c>
       <c r="B42" t="s">
         <v>100</v>
@@ -1827,12 +1795,12 @@
         <v>3</v>
       </c>
       <c r="E42">
-        <f t="shared" ca="1" si="1"/>
-        <v>6376928469</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5716679907</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3252295088</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3942810673</v>
       </c>
       <c r="G42" t="s">
         <v>4</v>
@@ -1840,8 +1808,7 @@
     </row>
     <row r="43" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43923</v>
       </c>
       <c r="B43" t="s">
         <v>101</v>
@@ -1853,12 +1820,12 @@
         <v>3</v>
       </c>
       <c r="E43">
-        <f t="shared" ca="1" si="1"/>
-        <v>5763593401</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3604145451</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3852436766</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3672501388</v>
       </c>
       <c r="G43" t="s">
         <v>38</v>
@@ -1866,8 +1833,7 @@
     </row>
     <row r="44" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43924</v>
       </c>
       <c r="B44" t="s">
         <v>102</v>
@@ -1879,12 +1845,12 @@
         <v>3</v>
       </c>
       <c r="E44">
-        <f t="shared" ca="1" si="1"/>
-        <v>8812131200</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5983240618</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3354562978</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3531652284</v>
       </c>
       <c r="G44" t="s">
         <v>6</v>
@@ -1892,8 +1858,7 @@
     </row>
     <row r="45" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43925</v>
       </c>
       <c r="B45" t="s">
         <v>103</v>
@@ -1905,12 +1870,12 @@
         <v>3</v>
       </c>
       <c r="E45">
-        <f t="shared" ca="1" si="1"/>
-        <v>2681130857</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6832342389</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3926495203</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3972735771</v>
       </c>
       <c r="G45" t="s">
         <v>39</v>
@@ -1918,8 +1883,7 @@
     </row>
     <row r="46" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43926</v>
       </c>
       <c r="B46" t="s">
         <v>104</v>
@@ -1931,12 +1895,12 @@
         <v>3</v>
       </c>
       <c r="E46">
-        <f t="shared" ca="1" si="1"/>
-        <v>653180009</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6304024082</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3390067327</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3648274398</v>
       </c>
       <c r="G46" t="s">
         <v>7</v>
@@ -1944,8 +1908,7 @@
     </row>
     <row r="47" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43927</v>
       </c>
       <c r="B47" t="s">
         <v>105</v>
@@ -1957,12 +1920,12 @@
         <v>3</v>
       </c>
       <c r="E47">
-        <f t="shared" ca="1" si="1"/>
-        <v>6173337666</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7831680700</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>338233932</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3377851136</v>
       </c>
       <c r="G47" t="s">
         <v>5</v>
@@ -1970,8 +1933,7 @@
     </row>
     <row r="48" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43928</v>
       </c>
       <c r="B48" t="s">
         <v>106</v>
@@ -1983,12 +1945,12 @@
         <v>3</v>
       </c>
       <c r="E48">
-        <f t="shared" ca="1" si="1"/>
-        <v>4379586803</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6119564562</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>314161341</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3545248860</v>
       </c>
       <c r="G48" t="s">
         <v>4</v>
@@ -1996,8 +1958,7 @@
     </row>
     <row r="49" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43929</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>81</v>
@@ -2009,12 +1970,12 @@
         <v>3</v>
       </c>
       <c r="E49">
-        <f t="shared" ca="1" si="1"/>
-        <v>2085484989</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>481249858</v>
       </c>
       <c r="F49" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3475292451</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3808297987</v>
       </c>
       <c r="G49" t="s">
         <v>38</v>
@@ -2022,8 +1983,7 @@
     </row>
     <row r="50" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43930</v>
       </c>
       <c r="B50" t="s">
         <v>107</v>
@@ -2035,12 +1995,12 @@
         <v>3</v>
       </c>
       <c r="E50">
-        <f t="shared" ca="1" si="1"/>
-        <v>8469382353</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6459167633</v>
       </c>
       <c r="F50" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3834187320</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3648443355</v>
       </c>
       <c r="G50" t="s">
         <v>4</v>
@@ -2048,8 +2008,7 @@
     </row>
     <row r="51" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43931</v>
       </c>
       <c r="B51" t="s">
         <v>108</v>
@@ -2061,12 +2020,12 @@
         <v>3</v>
       </c>
       <c r="E51">
-        <f t="shared" ca="1" si="1"/>
-        <v>7145068514</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7580395541</v>
       </c>
       <c r="F51" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3543787436</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3450567665</v>
       </c>
       <c r="G51" t="s">
         <v>38</v>
@@ -2074,8 +2033,7 @@
     </row>
     <row r="52" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43932</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>82</v>
@@ -2087,12 +2045,12 @@
         <v>3</v>
       </c>
       <c r="E52">
-        <f t="shared" ca="1" si="1"/>
-        <v>4947404582</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7161951758</v>
       </c>
       <c r="F52" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3958262719</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3634825406</v>
       </c>
       <c r="G52" t="s">
         <v>6</v>
@@ -2100,8 +2058,7 @@
     </row>
     <row r="53" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43933</v>
       </c>
       <c r="B53" t="s">
         <v>109</v>
@@ -2113,12 +2070,12 @@
         <v>3</v>
       </c>
       <c r="E53">
-        <f t="shared" ca="1" si="1"/>
-        <v>2152264420</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7619565411</v>
       </c>
       <c r="F53" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3857167077</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3510447102</v>
       </c>
       <c r="G53" t="s">
         <v>39</v>
@@ -2126,8 +2083,7 @@
     </row>
     <row r="54" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43934</v>
       </c>
       <c r="B54" t="s">
         <v>110</v>
@@ -2139,12 +2095,12 @@
         <v>3</v>
       </c>
       <c r="E54">
-        <f t="shared" ca="1" si="1"/>
-        <v>7276312916</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>155282303</v>
       </c>
       <c r="F54" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3704849098</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3336793916</v>
       </c>
       <c r="G54" t="s">
         <v>7</v>
@@ -2152,8 +2108,7 @@
     </row>
     <row r="55" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43935</v>
       </c>
       <c r="B55" t="s">
         <v>111</v>
@@ -2165,12 +2120,12 @@
         <v>3</v>
       </c>
       <c r="E55">
-        <f t="shared" ca="1" si="1"/>
-        <v>7551894404</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5405313801</v>
       </c>
       <c r="F55" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3202634534</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3431667706</v>
       </c>
       <c r="G55" t="s">
         <v>5</v>
@@ -2178,8 +2133,7 @@
     </row>
     <row r="56" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43936</v>
       </c>
       <c r="B56" t="s">
         <v>112</v>
@@ -2191,12 +2145,12 @@
         <v>3</v>
       </c>
       <c r="E56">
-        <f t="shared" ca="1" si="1"/>
-        <v>1091702375</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6771129763</v>
       </c>
       <c r="F56" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3360985502</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3861564521</v>
       </c>
       <c r="G56" t="s">
         <v>4</v>
@@ -2204,8 +2158,7 @@
     </row>
     <row r="57" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43937</v>
       </c>
       <c r="B57" t="s">
         <v>113</v>
@@ -2217,12 +2170,12 @@
         <v>3</v>
       </c>
       <c r="E57">
-        <f t="shared" ca="1" si="1"/>
-        <v>6260514936</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6063980129</v>
       </c>
       <c r="F57" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3995407587</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3492987434</v>
       </c>
       <c r="G57" t="s">
         <v>38</v>
@@ -2230,8 +2183,7 @@
     </row>
     <row r="58" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43938</v>
       </c>
       <c r="B58" t="s">
         <v>114</v>
@@ -2243,12 +2195,12 @@
         <v>3</v>
       </c>
       <c r="E58">
-        <f t="shared" ca="1" si="1"/>
-        <v>948374570</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3750393546</v>
       </c>
       <c r="F58" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3208685623</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3821499019</v>
       </c>
       <c r="G58" t="s">
         <v>4</v>
@@ -2256,8 +2208,7 @@
     </row>
     <row r="59" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43939</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>83</v>
@@ -2269,12 +2220,12 @@
         <v>3</v>
       </c>
       <c r="E59">
-        <f t="shared" ca="1" si="1"/>
-        <v>5482407084</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9772659634</v>
       </c>
       <c r="F59" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3553428714</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3444565751</v>
       </c>
       <c r="G59" t="s">
         <v>38</v>
@@ -2282,8 +2233,7 @@
     </row>
     <row r="60" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43941</v>
+        <v>43940</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>84</v>
@@ -2295,12 +2245,12 @@
         <v>3</v>
       </c>
       <c r="E60">
-        <f t="shared" ca="1" si="1"/>
-        <v>7017477318</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9289334218</v>
       </c>
       <c r="F60" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>3382046479</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>352995247</v>
       </c>
       <c r="G60" t="s">
         <v>6</v>
@@ -2309,7 +2259,9 @@
     <row r="61" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="62" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="63" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:7" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D64" s="8"/>
+    </row>
     <row r="65" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="66" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="67" ht="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>